<commit_message>
some tweaks to test 3 solutions
</commit_message>
<xml_diff>
--- a/2018_2019/Tests/Test 2 solutions/Test2_signatures.xlsx
+++ b/2018_2019/Tests/Test 2 solutions/Test2_signatures.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esther\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esther\Documents\GitHub\instruments-master\2018_2019\Tests\Test 2 solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="11685"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1688,7 +1688,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
   <headerFooter>
-    <oddHeader>&amp;CTest 2</oddHeader>
+    <oddHeader>&amp;CTest 3</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes to admin of test 4
</commit_message>
<xml_diff>
--- a/2018_2019/Tests/Test 2 solutions/Test2_signatures.xlsx
+++ b/2018_2019/Tests/Test 2 solutions/Test2_signatures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11685"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D70" sqref="A1:D70"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A41" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1688,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
   <headerFooter>
-    <oddHeader>&amp;CTest 3</oddHeader>
+    <oddHeader>&amp;CTest 4</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>